<commit_message>
Created a LoginDDT with the report file
</commit_message>
<xml_diff>
--- a/src/test/java/com/ebanking/testData/LoginData.xlsx
+++ b/src/test/java/com/ebanking/testData/LoginData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24859E2E-FA91-4B2E-B490-FEAA815333A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627139B1-F4F6-4141-A5D1-515358479ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,12 +78,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF569CD6"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -127,13 +121,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,12 +499,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>